<commit_message>
tilføjet alle opgs til samlet dokument
</commit_message>
<xml_diff>
--- a/MAL/02/mangler 02.xlsx
+++ b/MAL/02/mangler 02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\6-Semester\MAL\02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1925A34A-BE02-4274-A0AA-4363452B2DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C6AC2F-A984-43F8-A636-7BCB3F079F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C036A88A-9653-4D79-9F35-061B5BF208DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>L03 - Supergruppe diskussion</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Mangler alt</t>
   </si>
   <si>
-    <t>en masse spg</t>
-  </si>
-  <si>
     <t>L06 - ANN</t>
   </si>
   <si>
@@ -87,6 +84,33 @@
   </si>
   <si>
     <t>mangler, ændre nogle parametre blabla</t>
+  </si>
+  <si>
+    <t>mangler intro</t>
+  </si>
+  <si>
+    <t>mangler tekst</t>
+  </si>
+  <si>
+    <t>mangler kode/opgave</t>
+  </si>
+  <si>
+    <t>mangler forklaring</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>husk at indsæt nyt billede med endelig data THOMAS</t>
+  </si>
+  <si>
+    <t>mangler tekst, ryk kode op I markdown spørg lasse</t>
+  </si>
+  <si>
+    <t>graf er skæv, lav om???? Passer ikke</t>
+  </si>
+  <si>
+    <t>mangler kode, victoria har det</t>
   </si>
 </sst>
 </file>
@@ -496,134 +520,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A729BAE3-6EF1-4B60-8534-BA7C6D7CF7E4}">
-  <dimension ref="B2:C26"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="42.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>12</v>
+      <c r="C26" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Qa+b in pipelines
</commit_message>
<xml_diff>
--- a/MAL/02/mangler 02.xlsx
+++ b/MAL/02/mangler 02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\6-Semester\MAL\02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C6AC2F-A984-43F8-A636-7BCB3F079F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FD7516-9E2B-44B5-A52F-38C5C23C633C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C036A88A-9653-4D79-9F35-061B5BF208DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>L03 - Supergruppe diskussion</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Qf</t>
-  </si>
-  <si>
-    <t>Mangler kort forkalring</t>
   </si>
   <si>
     <t>mangler kort forklaring</t>
@@ -523,7 +520,7 @@
   <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,17 +542,17 @@
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -584,16 +581,14 @@
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -601,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
@@ -609,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
@@ -630,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -638,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -646,7 +641,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -654,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -662,7 +657,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -670,7 +665,7 @@
         <v>10</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -678,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Qabc i pipelines færdig
</commit_message>
<xml_diff>
--- a/MAL/02/mangler 02.xlsx
+++ b/MAL/02/mangler 02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\6-Semester\MAL\02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FD7516-9E2B-44B5-A52F-38C5C23C633C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC366C43-9267-470B-B449-74D83033AB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C036A88A-9653-4D79-9F35-061B5BF208DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>L03 - Supergruppe diskussion</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>Qf</t>
-  </si>
-  <si>
-    <t>mangler kort forklaring</t>
-  </si>
-  <si>
-    <t>mangler forklaring / svar på spg</t>
   </si>
   <si>
     <t>mangler, ændre nogle parametre blabla</t>
@@ -520,7 +514,7 @@
   <dimension ref="B2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,17 +536,17 @@
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -587,24 +581,20 @@
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
@@ -625,7 +615,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -633,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -641,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -649,7 +639,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -657,7 +647,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -665,7 +655,7 @@
         <v>10</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -673,7 +663,7 @@
         <v>11</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mangler kun konkl og ret billede
</commit_message>
<xml_diff>
--- a/MAL/02/mangler 02.xlsx
+++ b/MAL/02/mangler 02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\6-Semester\MAL\02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC366C43-9267-470B-B449-74D83033AB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC284B0-647E-4FD2-BF09-038B36465E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C036A88A-9653-4D79-9F35-061B5BF208DB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>L03 - Supergruppe diskussion</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>Qf</t>
-  </si>
-  <si>
-    <t>mangler, ændre nogle parametre blabla</t>
-  </si>
-  <si>
-    <t>mangler intro</t>
   </si>
   <si>
     <t>mangler tekst</t>
@@ -132,7 +126,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +151,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -170,13 +170,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A729BAE3-6EF1-4B60-8534-BA7C6D7CF7E4}">
   <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,17 +537,17 @@
       </c>
       <c r="C3" s="1"/>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -593,9 +594,7 @@
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C16" s="3" t="s">
@@ -606,7 +605,7 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -614,56 +613,54 @@
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>14</v>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>19</v>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>20</v>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>21</v>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>14</v>
+      <c r="C26" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>